<commit_message>
leaderboard ranking algorithm updated
</commit_message>
<xml_diff>
--- a/public/assets/data/leaderboard.xlsx
+++ b/public/assets/data/leaderboard.xlsx
@@ -2400,7 +2400,7 @@
         <v>0.0</v>
       </c>
       <c r="I4" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>17</v>
@@ -2435,7 +2435,7 @@
         <v>0.0</v>
       </c>
       <c r="I5" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>17</v>
@@ -2476,7 +2476,7 @@
         <v>17</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">
@@ -2499,13 +2499,13 @@
         <v>38</v>
       </c>
       <c r="G7" s="1">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H7" s="1">
         <v>0.0</v>
       </c>
       <c r="I7" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>17</v>
@@ -2540,13 +2540,13 @@
         <v>0.0</v>
       </c>
       <c r="I8" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9">
@@ -2575,13 +2575,13 @@
         <v>0.0</v>
       </c>
       <c r="I9" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
@@ -2645,13 +2645,13 @@
         <v>0.0</v>
       </c>
       <c r="I11" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
@@ -2715,7 +2715,7 @@
         <v>0.0</v>
       </c>
       <c r="I13" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>17</v>
@@ -2750,7 +2750,7 @@
         <v>0.0</v>
       </c>
       <c r="I14" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>17</v>
@@ -2814,7 +2814,7 @@
         <v>74</v>
       </c>
       <c r="G16" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H16" s="1">
         <v>0.0</v>
@@ -2925,7 +2925,7 @@
         <v>0.0</v>
       </c>
       <c r="I19" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>17</v>
@@ -3100,13 +3100,13 @@
         <v>0.0</v>
       </c>
       <c r="I24" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25">
@@ -3141,7 +3141,7 @@
         <v>17</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26">
@@ -3246,7 +3246,7 @@
         <v>17</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29">
@@ -3310,7 +3310,7 @@
         <v>0.0</v>
       </c>
       <c r="I30" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>17</v>
@@ -3421,7 +3421,7 @@
         <v>17</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34">
@@ -3514,13 +3514,13 @@
         <v>154</v>
       </c>
       <c r="G36" s="1">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H36" s="1">
         <v>0.0</v>
       </c>
       <c r="I36" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>17</v>
@@ -3625,7 +3625,7 @@
         <v>0.0</v>
       </c>
       <c r="I39" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>17</v>
@@ -3765,13 +3765,13 @@
         <v>0.0</v>
       </c>
       <c r="I43" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44">
@@ -3905,7 +3905,7 @@
         <v>0.0</v>
       </c>
       <c r="I47" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>17</v>
@@ -3975,7 +3975,7 @@
         <v>0.0</v>
       </c>
       <c r="I49" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J49" s="1" t="s">
         <v>17</v>
@@ -4080,7 +4080,7 @@
         <v>0.0</v>
       </c>
       <c r="I52" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>17</v>
@@ -4115,7 +4115,7 @@
         <v>0.0</v>
       </c>
       <c r="I53" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>17</v>
@@ -4144,19 +4144,19 @@
         <v>226</v>
       </c>
       <c r="G54" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H54" s="1">
         <v>0.0</v>
       </c>
       <c r="I54" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55">
@@ -4185,13 +4185,13 @@
         <v>0.0</v>
       </c>
       <c r="I55" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56">
@@ -4290,13 +4290,13 @@
         <v>0.0</v>
       </c>
       <c r="I58" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J58" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59">
@@ -4325,13 +4325,13 @@
         <v>0.0</v>
       </c>
       <c r="I59" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K59" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="60">
@@ -4395,7 +4395,7 @@
         <v>0.0</v>
       </c>
       <c r="I61" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J61" s="1" t="s">
         <v>17</v>
@@ -4430,7 +4430,7 @@
         <v>0.0</v>
       </c>
       <c r="I62" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J62" s="1" t="s">
         <v>17</v>
@@ -4500,13 +4500,13 @@
         <v>0.0</v>
       </c>
       <c r="I64" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J64" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K64" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="65">
@@ -4570,7 +4570,7 @@
         <v>0.0</v>
       </c>
       <c r="I66" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J66" s="1" t="s">
         <v>17</v>
@@ -4675,13 +4675,13 @@
         <v>0.0</v>
       </c>
       <c r="I69" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J69" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K69" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="70">
@@ -4780,7 +4780,7 @@
         <v>0.0</v>
       </c>
       <c r="I72" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J72" s="1" t="s">
         <v>17</v>
@@ -4815,13 +4815,13 @@
         <v>0.0</v>
       </c>
       <c r="I73" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J73" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K73" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="74">
@@ -4850,7 +4850,7 @@
         <v>0.0</v>
       </c>
       <c r="I74" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J74" s="1" t="s">
         <v>17</v>
@@ -4891,7 +4891,7 @@
         <v>17</v>
       </c>
       <c r="K75" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="76">
@@ -4920,7 +4920,7 @@
         <v>0.0</v>
       </c>
       <c r="I76" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J76" s="1" t="s">
         <v>17</v>
@@ -4955,7 +4955,7 @@
         <v>0.0</v>
       </c>
       <c r="I77" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J77" s="1" t="s">
         <v>17</v>
@@ -4984,13 +4984,13 @@
         <v>322</v>
       </c>
       <c r="G78" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H78" s="1">
         <v>0.0</v>
       </c>
       <c r="I78" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J78" s="1" t="s">
         <v>17</v>
@@ -5060,7 +5060,7 @@
         <v>0.0</v>
       </c>
       <c r="I80" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J80" s="1" t="s">
         <v>17</v>
@@ -5270,13 +5270,13 @@
         <v>0.0</v>
       </c>
       <c r="I86" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J86" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K86" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="87">
@@ -5311,7 +5311,7 @@
         <v>17</v>
       </c>
       <c r="K87" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="88">
@@ -5340,7 +5340,7 @@
         <v>0.0</v>
       </c>
       <c r="I88" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J88" s="1" t="s">
         <v>17</v>
@@ -5375,7 +5375,7 @@
         <v>0.0</v>
       </c>
       <c r="I89" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J89" s="1" t="s">
         <v>17</v>
@@ -5521,7 +5521,7 @@
         <v>17</v>
       </c>
       <c r="K93" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="94">
@@ -5550,7 +5550,7 @@
         <v>0.0</v>
       </c>
       <c r="I94" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J94" s="1" t="s">
         <v>17</v>
@@ -5585,7 +5585,7 @@
         <v>0.0</v>
       </c>
       <c r="I95" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J95" s="1" t="s">
         <v>17</v>
@@ -5620,13 +5620,13 @@
         <v>0.0</v>
       </c>
       <c r="I96" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J96" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K96" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="97">
@@ -5760,7 +5760,7 @@
         <v>0.0</v>
       </c>
       <c r="I100" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J100" s="1" t="s">
         <v>17</v>
@@ -5859,7 +5859,7 @@
         <v>423</v>
       </c>
       <c r="G103" s="1">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="H103" s="1">
         <v>0.0</v>
@@ -6104,19 +6104,19 @@
         <v>451</v>
       </c>
       <c r="G110" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H110" s="1">
         <v>0.0</v>
       </c>
       <c r="I110" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J110" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K110" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="111">
@@ -6139,19 +6139,19 @@
         <v>455</v>
       </c>
       <c r="G111" s="1">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="H111" s="1">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="I111" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J111" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K111" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="112">
@@ -6180,13 +6180,13 @@
         <v>0.0</v>
       </c>
       <c r="I112" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J112" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K112" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="113">
@@ -6495,13 +6495,13 @@
         <v>0.0</v>
       </c>
       <c r="I121" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J121" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="122">
@@ -6530,7 +6530,7 @@
         <v>0.0</v>
       </c>
       <c r="I122" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J122" s="1" t="s">
         <v>17</v>
@@ -6600,13 +6600,13 @@
         <v>0.0</v>
       </c>
       <c r="I124" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J124" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K124" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="125">
@@ -6635,13 +6635,13 @@
         <v>0.0</v>
       </c>
       <c r="I125" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J125" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K125" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="126">
@@ -6670,7 +6670,7 @@
         <v>0.0</v>
       </c>
       <c r="I126" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J126" s="1" t="s">
         <v>17</v>
@@ -6705,13 +6705,13 @@
         <v>0.0</v>
       </c>
       <c r="I127" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J127" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K127" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="128">
@@ -7020,7 +7020,7 @@
         <v>0.0</v>
       </c>
       <c r="I136" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J136" s="1" t="s">
         <v>17</v>
@@ -7055,7 +7055,7 @@
         <v>0.0</v>
       </c>
       <c r="I137" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J137" s="1" t="s">
         <v>17</v>
@@ -7265,7 +7265,7 @@
         <v>0.0</v>
       </c>
       <c r="I143" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J143" s="1" t="s">
         <v>17</v>
@@ -7329,7 +7329,7 @@
         <v>591</v>
       </c>
       <c r="G145" s="1">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H145" s="1">
         <v>0.0</v>
@@ -7510,7 +7510,7 @@
         <v>0.0</v>
       </c>
       <c r="I150" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J150" s="1" t="s">
         <v>17</v>
@@ -7650,7 +7650,7 @@
         <v>0.0</v>
       </c>
       <c r="I154" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J154" s="1" t="s">
         <v>17</v>
@@ -7755,7 +7755,7 @@
         <v>0.0</v>
       </c>
       <c r="I157" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J157" s="1" t="s">
         <v>17</v>
@@ -7790,7 +7790,7 @@
         <v>0.0</v>
       </c>
       <c r="I158" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J158" s="1" t="s">
         <v>17</v>
@@ -7860,7 +7860,7 @@
         <v>0.0</v>
       </c>
       <c r="I160" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J160" s="1" t="s">
         <v>17</v>
@@ -7895,7 +7895,7 @@
         <v>0.0</v>
       </c>
       <c r="I161" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J161" s="1" t="s">
         <v>17</v>
@@ -7971,7 +7971,7 @@
         <v>17</v>
       </c>
       <c r="K163" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="164">
@@ -8181,7 +8181,7 @@
         <v>17</v>
       </c>
       <c r="K169" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="170">
@@ -8210,7 +8210,7 @@
         <v>0.0</v>
       </c>
       <c r="I170" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J170" s="1" t="s">
         <v>17</v>
@@ -8315,7 +8315,7 @@
         <v>0.0</v>
       </c>
       <c r="I173" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J173" s="1" t="s">
         <v>17</v>
@@ -8350,7 +8350,7 @@
         <v>0.0</v>
       </c>
       <c r="I174" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J174" s="1" t="s">
         <v>17</v>
@@ -8455,7 +8455,7 @@
         <v>0.0</v>
       </c>
       <c r="I177" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J177" s="1" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
leaderboard update + ranking algo modification
</commit_message>
<xml_diff>
--- a/public/assets/data/leaderboard.xlsx
+++ b/public/assets/data/leaderboard.xlsx
@@ -2569,7 +2569,7 @@
         <v>46</v>
       </c>
       <c r="G9" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H9" s="1">
         <v>0.0</v>
@@ -2639,7 +2639,7 @@
         <v>54</v>
       </c>
       <c r="G11" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H11" s="1">
         <v>0.0</v>
@@ -2849,16 +2849,16 @@
         <v>78</v>
       </c>
       <c r="G17" s="1">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="H17" s="1">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="I17" s="1">
         <v>1.0</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>22</v>
@@ -3316,7 +3316,7 @@
         <v>17</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31">
@@ -3596,7 +3596,7 @@
         <v>17</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39">
@@ -3759,16 +3759,16 @@
         <v>182</v>
       </c>
       <c r="G43" s="1">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="H43" s="1">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="I43" s="1">
         <v>1.0</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>22</v>
@@ -4077,7 +4077,7 @@
         <v>0.0</v>
       </c>
       <c r="H52" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I52" s="1">
         <v>1.0</v>
@@ -4112,7 +4112,7 @@
         <v>0.0</v>
       </c>
       <c r="H53" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I53" s="1">
         <v>1.0</v>
@@ -4144,10 +4144,10 @@
         <v>226</v>
       </c>
       <c r="G54" s="1">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="H54" s="1">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="I54" s="1">
         <v>1.0</v>
@@ -4471,7 +4471,7 @@
         <v>17</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64">
@@ -5066,7 +5066,7 @@
         <v>17</v>
       </c>
       <c r="K80" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="81">
@@ -5305,7 +5305,7 @@
         <v>0.0</v>
       </c>
       <c r="I87" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="J87" s="1" t="s">
         <v>17</v>
@@ -5451,7 +5451,7 @@
         <v>17</v>
       </c>
       <c r="K91" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="92">
@@ -6081,7 +6081,7 @@
         <v>17</v>
       </c>
       <c r="K109" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="110">
@@ -6142,13 +6142,13 @@
         <v>4.0</v>
       </c>
       <c r="H111" s="1">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="I111" s="1">
         <v>1.0</v>
       </c>
       <c r="J111" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K111" s="1" t="s">
         <v>22</v>
@@ -6361,7 +6361,7 @@
         <v>17</v>
       </c>
       <c r="K117" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="118">
@@ -6524,7 +6524,7 @@
         <v>499</v>
       </c>
       <c r="G122" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H122" s="1">
         <v>0.0</v>
@@ -6536,7 +6536,7 @@
         <v>17</v>
       </c>
       <c r="K122" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="123">
@@ -6676,7 +6676,7 @@
         <v>17</v>
       </c>
       <c r="K126" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="127">
@@ -7259,7 +7259,7 @@
         <v>583</v>
       </c>
       <c r="G143" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H143" s="1">
         <v>0.0</v>
@@ -7271,7 +7271,7 @@
         <v>17</v>
       </c>
       <c r="K143" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="144">
@@ -7329,10 +7329,10 @@
         <v>591</v>
       </c>
       <c r="G145" s="1">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="H145" s="1">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="I145" s="1">
         <v>1.0</v>
@@ -7656,7 +7656,7 @@
         <v>17</v>
       </c>
       <c r="K154" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="155">
@@ -7866,7 +7866,7 @@
         <v>17</v>
       </c>
       <c r="K160" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="161">
@@ -8356,7 +8356,7 @@
         <v>17</v>
       </c>
       <c r="K174" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="175">

</xml_diff>

<commit_message>
leaderboard update; with search feature
</commit_message>
<xml_diff>
--- a/public/assets/data/leaderboard.xlsx
+++ b/public/assets/data/leaderboard.xlsx
@@ -2499,16 +2499,16 @@
         <v>38</v>
       </c>
       <c r="G7" s="1">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="H7" s="1">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="I7" s="1">
         <v>1.0</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>22</v>
@@ -2534,7 +2534,7 @@
         <v>42</v>
       </c>
       <c r="G8" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H8" s="1">
         <v>0.0</v>
@@ -2569,7 +2569,7 @@
         <v>46</v>
       </c>
       <c r="G9" s="1">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="H9" s="1">
         <v>0.0</v>
@@ -2639,16 +2639,16 @@
         <v>54</v>
       </c>
       <c r="G11" s="1">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="H11" s="1">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="I11" s="1">
         <v>1.0</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>22</v>
@@ -2814,16 +2814,16 @@
         <v>74</v>
       </c>
       <c r="G16" s="1">
-        <v>1.0</v>
+        <v>4.0</v>
       </c>
       <c r="H16" s="1">
-        <v>0.0</v>
+        <v>4.0</v>
       </c>
       <c r="I16" s="1">
         <v>1.0</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>22</v>
@@ -3094,7 +3094,7 @@
         <v>106</v>
       </c>
       <c r="G24" s="1">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="H24" s="1">
         <v>0.0</v>
@@ -3899,7 +3899,7 @@
         <v>198</v>
       </c>
       <c r="G47" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H47" s="1">
         <v>0.0</v>
@@ -3969,7 +3969,7 @@
         <v>206</v>
       </c>
       <c r="G49" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H49" s="1">
         <v>0.0</v>
@@ -4494,7 +4494,7 @@
         <v>266</v>
       </c>
       <c r="G64" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H64" s="1">
         <v>0.0</v>
@@ -4669,7 +4669,7 @@
         <v>286</v>
       </c>
       <c r="G69" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H69" s="1">
         <v>0.0</v>
@@ -4984,7 +4984,7 @@
         <v>322</v>
       </c>
       <c r="G78" s="1">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="H78" s="1">
         <v>0.0</v>
@@ -5241,7 +5241,7 @@
         <v>17</v>
       </c>
       <c r="K85" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="86">
@@ -5579,7 +5579,7 @@
         <v>390</v>
       </c>
       <c r="G95" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H95" s="1">
         <v>0.0</v>
@@ -5859,10 +5859,10 @@
         <v>423</v>
       </c>
       <c r="G103" s="1">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="H103" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I103" s="1">
         <v>1.0</v>
@@ -6104,10 +6104,10 @@
         <v>451</v>
       </c>
       <c r="G110" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="H110" s="1">
         <v>1.0</v>
-      </c>
-      <c r="H110" s="1">
-        <v>0.0</v>
       </c>
       <c r="I110" s="1">
         <v>1.0</v>
@@ -6527,7 +6527,7 @@
         <v>1.0</v>
       </c>
       <c r="H122" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I122" s="1">
         <v>1.0</v>
@@ -7061,7 +7061,7 @@
         <v>17</v>
       </c>
       <c r="K137" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="138">
@@ -7332,13 +7332,13 @@
         <v>4.0</v>
       </c>
       <c r="H145" s="1">
-        <v>3.0</v>
+        <v>4.0</v>
       </c>
       <c r="I145" s="1">
         <v>1.0</v>
       </c>
       <c r="J145" s="1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="K145" s="1" t="s">
         <v>22</v>
@@ -7539,10 +7539,10 @@
         <v>615</v>
       </c>
       <c r="G151" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H151" s="1">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="I151" s="1">
         <v>1.0</v>
@@ -8519,7 +8519,7 @@
         <v>726</v>
       </c>
       <c r="G179" s="1">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="H179" s="1">
         <v>0.0</v>

</xml_diff>